<commit_message>
bug fix and added logop
</commit_message>
<xml_diff>
--- a/LR1-Table.xlsx
+++ b/LR1-Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="657">
   <si>
     <t>State</t>
   </si>
@@ -2452,10 +2452,10 @@
   <dimension ref="A1:BR1577"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="BI692" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomRight" activeCell="BM699" sqref="BM699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8861,6 +8861,18 @@
       </c>
       <c r="B424" t="s">
         <v>363</v>
+      </c>
+      <c r="X424" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="Y424" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z424" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="AA424" s="7" t="s">
+        <v>311</v>
       </c>
       <c r="AF424" s="7" t="s">
         <v>311</v>
@@ -11266,26 +11278,26 @@
       <c r="BK699" s="4">
         <v>62</v>
       </c>
-      <c r="BL699" s="4">
-        <v>145</v>
-      </c>
-      <c r="BM699" s="4">
-        <v>145</v>
-      </c>
-      <c r="BN699" s="4">
-        <v>145</v>
-      </c>
-      <c r="BO699" s="4">
-        <v>145</v>
-      </c>
-      <c r="BP699" s="4">
-        <v>145</v>
-      </c>
-      <c r="BQ699" s="4">
-        <v>145</v>
-      </c>
-      <c r="BR699" s="4">
-        <v>145</v>
+      <c r="BL699" s="11">
+        <v>63</v>
+      </c>
+      <c r="BM699" s="11">
+        <v>64</v>
+      </c>
+      <c r="BN699" s="11">
+        <v>66</v>
+      </c>
+      <c r="BO699" s="11">
+        <v>67</v>
+      </c>
+      <c r="BP699" s="11">
+        <v>68</v>
+      </c>
+      <c r="BQ699" s="11">
+        <v>69</v>
+      </c>
+      <c r="BR699" s="11">
+        <v>71</v>
       </c>
     </row>
     <row r="700" spans="1:70" x14ac:dyDescent="0.25">
@@ -11685,19 +11697,19 @@
         <v>64</v>
       </c>
       <c r="BN755" s="4">
-        <v>147</v>
+        <v>66</v>
       </c>
       <c r="BO755" s="4">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="BP755" s="4">
-        <v>147</v>
+        <v>68</v>
       </c>
       <c r="BQ755" s="4">
-        <v>147</v>
+        <v>69</v>
       </c>
       <c r="BR755" s="4">
-        <v>147</v>
+        <v>71</v>
       </c>
     </row>
     <row r="756" spans="1:70" x14ac:dyDescent="0.25">
@@ -12855,8 +12867,8 @@
       <c r="BQ900">
         <v>69</v>
       </c>
-      <c r="BR900">
-        <v>156</v>
+      <c r="BR900" s="7">
+        <v>71</v>
       </c>
     </row>
     <row r="901" spans="1:70" x14ac:dyDescent="0.25">
@@ -14362,6 +14374,18 @@
       </c>
       <c r="B1093" t="s">
         <v>481</v>
+      </c>
+      <c r="X1093" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="Y1093" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="Z1093" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="AA1093" s="7" t="s">
+        <v>595</v>
       </c>
       <c r="AG1093" t="s">
         <v>354</v>

</xml_diff>